<commit_message>
Update the test cases spreadsheet with the latest test data and scenarios.
</commit_message>
<xml_diff>
--- a/IT23257054 TestCases.xlsx
+++ b/IT23257054 TestCases.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SLIIT\Y3S2\Assinment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B419F893-C688-487B-B1DF-DCC888B99F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AD403C-DF72-49B3-B166-340F45D0B9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{14655C8C-63A7-4A34-8F4F-718C9EB73A5A}"/>
   </bookViews>
   <sheets>
     <sheet name="test_cases" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">test_cases!$A$1:$I$41</definedName>
@@ -974,7 +973,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -990,19 +989,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1017,14 +1022,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1032,7 +1034,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1045,27 +1053,35 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1121,7 +1137,7 @@
     <tableColumn id="9" xr3:uid="{0F460C68-2CD5-4FF9-B4A5-E77237C63305}" uniqueName="9" name="Accuracy Justification / Issue Description" queryTableFieldId="9" dataDxfId="1"/>
     <tableColumn id="10" xr3:uid="{79924D07-C61F-4C8C-8BBE-2B74BFF30390}" uniqueName="10" name="What is covered by the test" queryTableFieldId="10" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1424,21 +1440,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F027FF-56AC-4236-BE94-07887FD85E21}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="11" zoomScaleNormal="22" workbookViewId="0">
-      <selection activeCell="AZ14" sqref="AZ14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="71" zoomScaleNormal="22" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.33203125" customWidth="1"/>
+    <col min="5" max="5" width="63" customWidth="1"/>
     <col min="6" max="6" width="77.6640625" customWidth="1"/>
     <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="80.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="113.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1448,7 +1464,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1471,28 +1487,28 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -1500,28 +1516,28 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1529,28 +1545,28 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1558,28 +1574,28 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="3" t="s">
         <v>31</v>
       </c>
       <c r="I5" s="2" t="s">
@@ -1587,28 +1603,28 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1616,28 +1632,28 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1645,28 +1661,28 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -1674,28 +1690,28 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="3" t="s">
         <v>49</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -1703,28 +1719,28 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="3" t="s">
         <v>54</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -1732,28 +1748,28 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="3" t="s">
         <v>59</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -1761,28 +1777,28 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>64</v>
       </c>
       <c r="I12" s="2" t="s">
@@ -1790,28 +1806,28 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>69</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -1819,28 +1835,28 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>74</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -1848,28 +1864,28 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>79</v>
       </c>
       <c r="I15" s="2" t="s">
@@ -1877,28 +1893,28 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>84</v>
       </c>
       <c r="I16" s="2" t="s">
@@ -1906,28 +1922,28 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>89</v>
       </c>
       <c r="I17" s="2" t="s">
@@ -1935,28 +1951,28 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>94</v>
       </c>
       <c r="I18" s="2" t="s">
@@ -1964,28 +1980,28 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="3" t="s">
         <v>99</v>
       </c>
       <c r="I19" s="2" t="s">
@@ -1993,28 +2009,28 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="3" t="s">
         <v>104</v>
       </c>
       <c r="I20" s="2" t="s">
@@ -2022,28 +2038,28 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="3" t="s">
         <v>109</v>
       </c>
       <c r="I21" s="2" t="s">
@@ -2051,28 +2067,28 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="3" t="s">
         <v>114</v>
       </c>
       <c r="I22" s="2" t="s">
@@ -2080,28 +2096,28 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="C23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="3" t="s">
         <v>119</v>
       </c>
       <c r="I23" s="2" t="s">
@@ -2109,28 +2125,28 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="C24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="3" t="s">
         <v>125</v>
       </c>
       <c r="I24" s="2" t="s">
@@ -2138,28 +2154,28 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="3" t="s">
         <v>130</v>
       </c>
       <c r="I25" s="2" t="s">
@@ -2167,28 +2183,28 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="4" t="s">
+      <c r="C26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="H26" s="3" t="s">
         <v>135</v>
       </c>
       <c r="I26" s="2" t="s">
@@ -2196,28 +2212,28 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="C27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="H27" s="3" t="s">
         <v>140</v>
       </c>
       <c r="I27" s="2" t="s">
@@ -2225,28 +2241,28 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="5" t="s">
+      <c r="C28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="3" t="s">
         <v>144</v>
       </c>
       <c r="I28" s="2" t="s">
@@ -2254,28 +2270,28 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="3" t="s">
         <v>149</v>
       </c>
       <c r="I29" s="2" t="s">
@@ -2283,28 +2299,28 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="C30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" s="3" t="s">
         <v>154</v>
       </c>
       <c r="I30" s="2" t="s">
@@ -2312,28 +2328,28 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="4" t="s">
+      <c r="C31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="3" t="s">
         <v>159</v>
       </c>
       <c r="I31" s="2" t="s">
@@ -2341,28 +2357,28 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="4" t="s">
+      <c r="C32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="H32" s="3" t="s">
         <v>164</v>
       </c>
       <c r="I32" s="2" t="s">
@@ -2370,28 +2386,28 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="C33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="H33" s="3" t="s">
         <v>169</v>
       </c>
       <c r="I33" s="2" t="s">
@@ -2399,28 +2415,28 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="C34" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="H34" s="3" t="s">
         <v>174</v>
       </c>
       <c r="I34" s="2" t="s">
@@ -2428,28 +2444,28 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="4" t="s">
+      <c r="C35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F35" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="H35" s="3" t="s">
         <v>179</v>
       </c>
       <c r="I35" s="2" t="s">
@@ -2457,28 +2473,28 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="4" t="s">
+      <c r="C36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="F36" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="H36" s="3" t="s">
         <v>184</v>
       </c>
       <c r="I36" s="2" t="s">
@@ -2486,28 +2502,28 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="F37" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="H37" s="3" t="s">
         <v>189</v>
       </c>
       <c r="I37" s="2" t="s">
@@ -2515,28 +2531,28 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="4" t="s">
+      <c r="C38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F38" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="G38" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H38" s="4" t="s">
+      <c r="H38" s="3" t="s">
         <v>194</v>
       </c>
       <c r="I38" s="2" t="s">
@@ -2544,28 +2560,28 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="4" t="s">
+      <c r="C39" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="G39" s="4" t="s">
+      <c r="G39" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H39" s="4" t="s">
+      <c r="H39" s="3" t="s">
         <v>199</v>
       </c>
       <c r="I39" s="2" t="s">
@@ -2573,28 +2589,28 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="C40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="F40" s="6" t="s">
+      <c r="F40" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G40" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="H40" s="3" t="s">
         <v>204</v>
       </c>
       <c r="I40" s="2" t="s">
@@ -2602,28 +2618,28 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="4" t="s">
+      <c r="C41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="3" t="s">
         <v>207</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="H41" s="3" t="s">
         <v>208</v>
       </c>
       <c r="I41" s="2" t="s">
@@ -2635,18 +2651,6 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0EF2DA-D666-46E9-8114-E70B8BF37F12}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>